<commit_message>
Scripting DPLKINV002-001, DPLKINV002-002 and DPLKINV002-028 until DPLKINV002-030
</commit_message>
<xml_diff>
--- a/DPLKINV002-001 -  Investasi - Reksadana - Entry Harga Pasar Upload Data/Report/Report/Default.xlsx
+++ b/DPLKINV002-001 -  Investasi - Reksadana - Entry Harga Pasar Upload Data/Report/Report/Default.xlsx
@@ -211,6 +211,9 @@
     <t>AB</t>
   </si>
   <si>
+    <t>http://192.168.168.111/</t>
+  </si>
+  <si>
     <t>AUTHOR</t>
   </si>
   <si>
@@ -233,9 +236,6 @@
   </si>
   <si>
     <t>AJ</t>
-  </si>
-  <si>
-    <t>http://192.168.168.107/</t>
   </si>
   <si>
     <t>Automation Tester 1</t>
@@ -620,68 +620,68 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -990,30 +990,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.078125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.078125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
@@ -1033,7 +1033,7 @@
         <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
@@ -1066,7 +1066,7 @@
         <v>103</v>
       </c>
       <c r="Q1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R1" t="s">
         <v>50</v>
@@ -1078,7 +1078,7 @@
         <v>23</v>
       </c>
       <c r="U1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V1" t="s">
         <v>95</v>
@@ -1106,14 +1106,14 @@
       <c r="C2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>71</v>
+      <c r="D2" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>35</v>
@@ -1158,7 +1158,7 @@
       <c r="Y2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="15"/>
+      <c r="Z2" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1174,33 +1174,33 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A7" sqref="A7:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.078125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.078125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
@@ -1296,26 +1296,26 @@
       <c r="I2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="19">
         <v>44896</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="N2" s="4"/>
-      <c r="O2" s="11"/>
+      <c r="O2" s="23"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="22"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="2"/>
@@ -1327,18 +1327,18 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="14"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="2"/>
       <c r="L3" s="4"/>
       <c r="M3" s="2"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="11"/>
+      <c r="O3" s="23"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="17"/>
+      <c r="U3" s="11"/>
     </row>
     <row r="4" ht="15">
       <c r="A4" s="2"/>
@@ -1350,18 +1350,18 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="2"/>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="11"/>
+      <c r="O4" s="23"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="2"/>
-      <c r="U4" s="17"/>
+      <c r="U4" s="11"/>
     </row>
     <row r="5" ht="15">
       <c r="A5" s="2"/>
@@ -1373,22 +1373,22 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="2"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="23"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="2"/>
-      <c r="U5" s="17"/>
+      <c r="U5" s="11"/>
     </row>
     <row r="6" ht="15">
       <c r="A6" s="2"/>
-      <c r="B6" s="12"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1407,11 +1407,11 @@
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="17"/>
+      <c r="U6" s="11"/>
     </row>
     <row r="7" ht="15">
       <c r="A7" s="2"/>
-      <c r="B7" s="12"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1430,7 +1430,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="17"/>
+      <c r="U7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1448,7 +1448,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="9" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -1467,49 +1467,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="9.078125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.140625" style="16" customWidth="1"/>
-    <col min="13" max="14" width="61" style="16" customWidth="1"/>
-    <col min="15" max="15" width="47" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="103.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="61" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="51" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="49.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="59.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="53.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="56.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="51.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="57.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="35.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.078125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.078125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.140625" style="25" customWidth="1"/>
+    <col min="13" max="14" width="61" style="25" customWidth="1"/>
+    <col min="15" max="15" width="47" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="103.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="69.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="61" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="63.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="51" style="25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="49.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="59.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="53.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="56.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="57.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="58.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="62.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="51.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="57.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="53.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="58.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.078125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
@@ -1538,7 +1538,7 @@
         <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J1" t="s">
         <v>33</v>
@@ -1547,7 +1547,7 @@
         <v>61</v>
       </c>
       <c r="L1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
         <v>97</v>
@@ -1607,7 +1607,7 @@
         <v>38</v>
       </c>
       <c r="AF1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AG1" t="s">
         <v>98</v>
@@ -1619,7 +1619,7 @@
         <v>39</v>
       </c>
       <c r="AJ1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AK1" t="s">
         <v>99</v>
@@ -1667,11 +1667,11 @@
         <v>Verifikasi Database DPLK</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
         <v>22</v>
@@ -1687,7 +1687,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="13"/>
+      <c r="V2" s="24"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -1711,7 +1711,7 @@
       <c r="AQ2" s="8"/>
       <c r="AR2" s="8"/>
       <c r="AS2" s="8"/>
-      <c r="AT2" s="25"/>
+      <c r="AT2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>